<commit_message>
Updated LoadRunner Ten\Fifteen summary
</commit_message>
<xml_diff>
--- a/Reports/Results/HearingRunResults.xlsx
+++ b/Reports/Results/HearingRunResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarav\Desktop\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarav\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889A447A-D4D1-41F7-9C5C-F5C1094E8D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E532A1-6C95-4F19-B819-96F49C3D25E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46DF73B-76A8-46F2-8740-0E9330EFA7B8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>35+</t>
+  </si>
+  <si>
+    <t>&lt;70</t>
+  </si>
+  <si>
+    <t>40+</t>
+  </si>
+  <si>
+    <t>70+</t>
+  </si>
+  <si>
+    <t>30+</t>
+  </si>
+  <si>
+    <t>&lt;60</t>
+  </si>
+  <si>
+    <t>LoadRunner</t>
   </si>
 </sst>
 </file>
@@ -473,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CFFF13-1140-453E-ACEC-DAD749A0C489}">
-  <dimension ref="B3:L13"/>
+  <dimension ref="B3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,10 +504,11 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="4"/>
+    <col min="10" max="10" width="12.42578125" style="4" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -515,16 +534,19 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>44077</v>
       </c>
@@ -549,11 +571,14 @@
       <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>44078</v>
       </c>
@@ -578,17 +603,20 @@
       <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>44081</v>
       </c>
@@ -613,11 +641,14 @@
       <c r="I6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>44081</v>
       </c>
@@ -642,17 +673,20 @@
       <c r="I7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>44081</v>
       </c>
@@ -677,11 +711,14 @@
       <c r="I8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>44082</v>
       </c>
@@ -706,17 +743,20 @@
       <c r="I9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>44082</v>
       </c>
@@ -741,17 +781,20 @@
       <c r="I10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>44083</v>
       </c>
@@ -776,17 +819,20 @@
       <c r="I11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>44089</v>
       </c>
@@ -811,17 +857,20 @@
       <c r="I12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>44089</v>
       </c>
@@ -846,14 +895,169 @@
       <c r="I13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="4">
         <v>70</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>44095</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="E14" s="3">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>44095</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E15" s="3">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>44097</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E16" s="3">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>44097</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E17" s="3">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="4">
+        <v>80</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>